<commit_message>
fixed diary AcceptanceDateAndTime and RequestDate
</commit_message>
<xml_diff>
--- a/Files/Templates/RequestTemplate.xlsx
+++ b/Files/Templates/RequestTemplate.xlsx
@@ -40,7 +40,7 @@
     <t>Срок за изпитване: #D дни</t>
   </si>
   <si>
-    <t>ЗАЯВКА № #NUMBER / Дата #DATE</t>
+    <t>ЗАЯВКА № #NUMBER / Дата #DATE / Час #TIME</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>